<commit_message>
Optimizations, more comments, updating formulas
User can now change specific pre-defined fields in each sheet, and the
changes they make will reflect in the “totals” section.
</commit_message>
<xml_diff>
--- a/test_file2.xlsx
+++ b/test_file2.xlsx
@@ -419,13 +419,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,8 +861,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5">
-        <v>84.1</v>
+      <c r="B5" s="2">
+        <f>SUM(C12,C13)</f>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>197</v>
@@ -911,7 +915,7 @@
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>82.6</v>
       </c>
       <c r="D12">
@@ -925,7 +929,7 @@
       <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>1.5</v>
       </c>
       <c r="D13">
@@ -940,15 +944,15 @@
         <v>34</v>
       </c>
       <c r="C14" s="2">
-        <f>SUM(C13:C12)</f>
+        <f>SUM(C12,C13)</f>
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <f>SUM(D13:D12)</f>
+        <f>SUM(D12,D13)</f>
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <f>SUM(E13:E12)</f>
+        <f>SUM(E12,E13)</f>
         <v>0</v>
       </c>
     </row>
@@ -972,8 +976,9 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="B19">
-        <v>143.5</v>
+      <c r="B19" s="2">
+        <f>SUM(C26)</f>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>213</v>
@@ -1025,7 +1030,7 @@
       <c r="B26" t="s">
         <v>38</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>143.5</v>
       </c>
       <c r="D26">
@@ -1040,15 +1045,15 @@
         <v>34</v>
       </c>
       <c r="C27" s="2">
-        <f>SUM(C26:C26)</f>
+        <f>SUM(C26)</f>
         <v>0</v>
       </c>
       <c r="D27" s="2">
-        <f>SUM(D26:D26)</f>
+        <f>SUM(D26)</f>
         <v>0</v>
       </c>
       <c r="E27" s="2">
-        <f>SUM(E26:E26)</f>
+        <f>SUM(E26)</f>
         <v>0</v>
       </c>
     </row>
@@ -1072,8 +1077,9 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32">
-        <v>35</v>
+      <c r="B32" s="2">
+        <f>SUM(C39)</f>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>199</v>
@@ -1125,7 +1131,7 @@
       <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <v>35</v>
       </c>
       <c r="D39">
@@ -1140,15 +1146,15 @@
         <v>34</v>
       </c>
       <c r="C40" s="2">
-        <f>SUM(C39:C39)</f>
+        <f>SUM(C39)</f>
         <v>0</v>
       </c>
       <c r="D40" s="2">
-        <f>SUM(D39:D39)</f>
+        <f>SUM(D39)</f>
         <v>0</v>
       </c>
       <c r="E40" s="2">
-        <f>SUM(E39:E39)</f>
+        <f>SUM(E39)</f>
         <v>0</v>
       </c>
     </row>
@@ -1172,8 +1178,9 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="B45">
-        <v>145.02</v>
+      <c r="B45" s="2">
+        <f>SUM(C52)</f>
+        <v>0</v>
       </c>
       <c r="C45">
         <v>190</v>
@@ -1225,7 +1232,7 @@
       <c r="B52" t="s">
         <v>44</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="3">
         <v>145.02</v>
       </c>
       <c r="D52">
@@ -1240,15 +1247,15 @@
         <v>34</v>
       </c>
       <c r="C53" s="2">
-        <f>SUM(C52:C52)</f>
+        <f>SUM(C52)</f>
         <v>0</v>
       </c>
       <c r="D53" s="2">
-        <f>SUM(D52:D52)</f>
+        <f>SUM(D52)</f>
         <v>0</v>
       </c>
       <c r="E53" s="2">
-        <f>SUM(E52:E52)</f>
+        <f>SUM(E52)</f>
         <v>0</v>
       </c>
     </row>
@@ -1272,8 +1279,9 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="B58">
-        <v>154.5</v>
+      <c r="B58" s="2">
+        <f>SUM(C65)</f>
+        <v>0</v>
       </c>
       <c r="C58">
         <v>194</v>
@@ -1325,7 +1333,7 @@
       <c r="B65" t="s">
         <v>47</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="3">
         <v>154.5</v>
       </c>
       <c r="D65">
@@ -1340,15 +1348,15 @@
         <v>34</v>
       </c>
       <c r="C66" s="2">
-        <f>SUM(C65:C65)</f>
+        <f>SUM(C65)</f>
         <v>0</v>
       </c>
       <c r="D66" s="2">
-        <f>SUM(D65:D65)</f>
+        <f>SUM(D65)</f>
         <v>0</v>
       </c>
       <c r="E66" s="2">
-        <f>SUM(E65:E65)</f>
+        <f>SUM(E65)</f>
         <v>0</v>
       </c>
     </row>
@@ -1372,8 +1380,9 @@
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="B71">
-        <v>449</v>
+      <c r="B71" s="2">
+        <f>SUM(C78,C79)</f>
+        <v>0</v>
       </c>
       <c r="C71">
         <v>198</v>
@@ -1425,7 +1434,7 @@
       <c r="B78" t="s">
         <v>50</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="3">
         <v>309</v>
       </c>
       <c r="D78">
@@ -1439,7 +1448,7 @@
       <c r="B79" t="s">
         <v>51</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="3">
         <v>140</v>
       </c>
       <c r="D79">
@@ -1454,15 +1463,15 @@
         <v>34</v>
       </c>
       <c r="C80" s="2">
-        <f>SUM(C79:C78)</f>
+        <f>SUM(C78,C79)</f>
         <v>0</v>
       </c>
       <c r="D80" s="2">
-        <f>SUM(D79:D78)</f>
+        <f>SUM(D78,D79)</f>
         <v>0</v>
       </c>
       <c r="E80" s="2">
-        <f>SUM(E79:E78)</f>
+        <f>SUM(E78,E79)</f>
         <v>0</v>
       </c>
     </row>
@@ -1486,8 +1495,9 @@
       </c>
     </row>
     <row r="85" spans="1:5">
-      <c r="B85">
-        <v>305.24</v>
+      <c r="B85" s="2">
+        <f>SUM(C92,C93,C94)</f>
+        <v>0</v>
       </c>
       <c r="C85">
         <v>192</v>
@@ -1539,7 +1549,7 @@
       <c r="B92" t="s">
         <v>54</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="3">
         <v>128.1</v>
       </c>
       <c r="D92">
@@ -1553,7 +1563,7 @@
       <c r="B93" t="s">
         <v>55</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="3">
         <v>53.64</v>
       </c>
       <c r="D93">
@@ -1567,7 +1577,7 @@
       <c r="B94" t="s">
         <v>56</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="3">
         <v>123.5</v>
       </c>
       <c r="D94">
@@ -1582,15 +1592,15 @@
         <v>34</v>
       </c>
       <c r="C95" s="2">
-        <f>SUM(C94:C92)</f>
+        <f>SUM(C92,C93,C94)</f>
         <v>0</v>
       </c>
       <c r="D95" s="2">
-        <f>SUM(D94:D92)</f>
+        <f>SUM(D92,D93,D94)</f>
         <v>0</v>
       </c>
       <c r="E95" s="2">
-        <f>SUM(E94:E92)</f>
+        <f>SUM(E92,E93,E94)</f>
         <v>0</v>
       </c>
     </row>
@@ -1614,8 +1624,9 @@
       </c>
     </row>
     <row r="100" spans="1:5">
-      <c r="B100">
-        <v>486.73</v>
+      <c r="B100" s="2">
+        <f>SUM(C107,C108,C109)</f>
+        <v>0</v>
       </c>
       <c r="C100">
         <v>177</v>
@@ -1667,7 +1678,7 @@
       <c r="B107" t="s">
         <v>59</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="3">
         <v>280.88</v>
       </c>
       <c r="D107">
@@ -1681,7 +1692,7 @@
       <c r="B108" t="s">
         <v>60</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="3">
         <v>73.85</v>
       </c>
       <c r="D108">
@@ -1695,7 +1706,7 @@
       <c r="B109" t="s">
         <v>61</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="3">
         <v>132</v>
       </c>
       <c r="D109">
@@ -1710,15 +1721,15 @@
         <v>34</v>
       </c>
       <c r="C110" s="2">
-        <f>SUM(C109:C107)</f>
+        <f>SUM(C107,C108,C109)</f>
         <v>0</v>
       </c>
       <c r="D110" s="2">
-        <f>SUM(D109:D107)</f>
+        <f>SUM(D107,D108,D109)</f>
         <v>0</v>
       </c>
       <c r="E110" s="2">
-        <f>SUM(E109:E107)</f>
+        <f>SUM(E107,E108,E109)</f>
         <v>0</v>
       </c>
     </row>
@@ -1742,8 +1753,9 @@
       </c>
     </row>
     <row r="115" spans="1:5">
-      <c r="B115">
-        <v>668.2</v>
+      <c r="B115" s="2">
+        <f>SUM(C122,C123,C124,C125,C126,C127)</f>
+        <v>0</v>
       </c>
       <c r="C115">
         <v>200</v>
@@ -1795,7 +1807,7 @@
       <c r="B122" t="s">
         <v>65</v>
       </c>
-      <c r="C122">
+      <c r="C122" s="3">
         <v>70</v>
       </c>
       <c r="D122">
@@ -1809,7 +1821,7 @@
       <c r="B123" t="s">
         <v>66</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="3">
         <v>147</v>
       </c>
       <c r="D123">
@@ -1823,7 +1835,7 @@
       <c r="B124" t="s">
         <v>67</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="3">
         <v>214</v>
       </c>
       <c r="D124">
@@ -1837,7 +1849,7 @@
       <c r="B125" t="s">
         <v>68</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="3">
         <v>183</v>
       </c>
       <c r="D125">
@@ -1851,7 +1863,7 @@
       <c r="B126" t="s">
         <v>69</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="3">
         <v>3</v>
       </c>
       <c r="D126">
@@ -1865,7 +1877,7 @@
       <c r="B127" t="s">
         <v>70</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="3">
         <v>51.2</v>
       </c>
       <c r="D127">
@@ -1880,15 +1892,15 @@
         <v>34</v>
       </c>
       <c r="C128" s="2">
-        <f>SUM(C127:C122)</f>
+        <f>SUM(C122,C123,C124,C125,C126,C127)</f>
         <v>0</v>
       </c>
       <c r="D128" s="2">
-        <f>SUM(D127:D122)</f>
+        <f>SUM(D122,D123,D124,D125,D126,D127)</f>
         <v>0</v>
       </c>
       <c r="E128" s="2">
-        <f>SUM(E127:E122)</f>
+        <f>SUM(E122,E123,E124,E125,E126,E127)</f>
         <v>0</v>
       </c>
     </row>
@@ -1912,8 +1924,9 @@
       </c>
     </row>
     <row r="133" spans="1:5">
-      <c r="B133">
-        <v>147.2</v>
+      <c r="B133" s="2">
+        <f>SUM(C140)</f>
+        <v>0</v>
       </c>
       <c r="C133">
         <v>216</v>
@@ -1965,7 +1978,7 @@
       <c r="B140" t="s">
         <v>73</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="3">
         <v>147.2</v>
       </c>
       <c r="D140">
@@ -1980,15 +1993,15 @@
         <v>34</v>
       </c>
       <c r="C141" s="2">
-        <f>SUM(C140:C140)</f>
+        <f>SUM(C140)</f>
         <v>0</v>
       </c>
       <c r="D141" s="2">
-        <f>SUM(D140:D140)</f>
+        <f>SUM(D140)</f>
         <v>0</v>
       </c>
       <c r="E141" s="2">
-        <f>SUM(E140:E140)</f>
+        <f>SUM(E140)</f>
         <v>0</v>
       </c>
     </row>
@@ -2012,8 +2025,9 @@
       </c>
     </row>
     <row r="146" spans="1:5">
-      <c r="B146">
-        <v>137.6</v>
+      <c r="B146" s="2">
+        <f>SUM(C153)</f>
+        <v>0</v>
       </c>
       <c r="C146">
         <v>198</v>
@@ -2065,7 +2079,7 @@
       <c r="B153" t="s">
         <v>75</v>
       </c>
-      <c r="C153">
+      <c r="C153" s="3">
         <v>137.6</v>
       </c>
       <c r="D153">
@@ -2080,15 +2094,15 @@
         <v>34</v>
       </c>
       <c r="C154" s="2">
-        <f>SUM(C153:C153)</f>
+        <f>SUM(C153)</f>
         <v>0</v>
       </c>
       <c r="D154" s="2">
-        <f>SUM(D153:D153)</f>
+        <f>SUM(D153)</f>
         <v>0</v>
       </c>
       <c r="E154" s="2">
-        <f>SUM(E153:E153)</f>
+        <f>SUM(E153)</f>
         <v>0</v>
       </c>
     </row>
@@ -2112,8 +2126,9 @@
       </c>
     </row>
     <row r="159" spans="1:5">
-      <c r="B159">
-        <v>134.5</v>
+      <c r="B159" s="2">
+        <f>SUM(C166)</f>
+        <v>0</v>
       </c>
       <c r="C159">
         <v>200</v>
@@ -2165,7 +2180,7 @@
       <c r="B166" t="s">
         <v>77</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="3">
         <v>134.5</v>
       </c>
       <c r="D166">
@@ -2180,15 +2195,15 @@
         <v>34</v>
       </c>
       <c r="C167" s="2">
-        <f>SUM(C166:C166)</f>
+        <f>SUM(C166)</f>
         <v>0</v>
       </c>
       <c r="D167" s="2">
-        <f>SUM(D166:D166)</f>
+        <f>SUM(D166)</f>
         <v>0</v>
       </c>
       <c r="E167" s="2">
-        <f>SUM(E166:E166)</f>
+        <f>SUM(E166)</f>
         <v>0</v>
       </c>
     </row>
@@ -2242,8 +2257,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5">
-        <v>84.1</v>
+      <c r="B5" s="2">
+        <f>SUM(C12,C13)</f>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>236.4</v>
@@ -2307,7 +2323,7 @@
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>82.6</v>
       </c>
       <c r="D12">
@@ -2321,7 +2337,7 @@
       <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>1.5</v>
       </c>
       <c r="D13">
@@ -2336,15 +2352,15 @@
         <v>34</v>
       </c>
       <c r="C14" s="2">
-        <f>SUM(C13:C12)</f>
+        <f>SUM(C12,C13)</f>
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <f>SUM(D13:D12)</f>
+        <f>SUM(D12,D13)</f>
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <f>SUM(E13:E12)</f>
+        <f>SUM(E12,E13)</f>
         <v>0</v>
       </c>
     </row>
@@ -2368,8 +2384,9 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="B19">
-        <v>143.5</v>
+      <c r="B19" s="2">
+        <f>SUM(C26)</f>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>255.6</v>
@@ -2433,7 +2450,7 @@
       <c r="B26" t="s">
         <v>38</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>143.5</v>
       </c>
       <c r="D26">
@@ -2448,15 +2465,15 @@
         <v>34</v>
       </c>
       <c r="C27" s="2">
-        <f>SUM(C26:C26)</f>
+        <f>SUM(C26)</f>
         <v>0</v>
       </c>
       <c r="D27" s="2">
-        <f>SUM(D26:D26)</f>
+        <f>SUM(D26)</f>
         <v>0</v>
       </c>
       <c r="E27" s="2">
-        <f>SUM(E26:E26)</f>
+        <f>SUM(E26)</f>
         <v>0</v>
       </c>
     </row>
@@ -2480,8 +2497,9 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="B32">
-        <v>35</v>
+      <c r="B32" s="2">
+        <f>SUM(C39)</f>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>238.8</v>
@@ -2545,7 +2563,7 @@
       <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <v>35</v>
       </c>
       <c r="D39">
@@ -2560,15 +2578,15 @@
         <v>34</v>
       </c>
       <c r="C40" s="2">
-        <f>SUM(C39:C39)</f>
+        <f>SUM(C39)</f>
         <v>0</v>
       </c>
       <c r="D40" s="2">
-        <f>SUM(D39:D39)</f>
+        <f>SUM(D39)</f>
         <v>0</v>
       </c>
       <c r="E40" s="2">
-        <f>SUM(E39:E39)</f>
+        <f>SUM(E39)</f>
         <v>0</v>
       </c>
     </row>
@@ -2592,8 +2610,9 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="B45">
-        <v>145.02</v>
+      <c r="B45" s="2">
+        <f>SUM(C52)</f>
+        <v>0</v>
       </c>
       <c r="C45">
         <v>228</v>
@@ -2657,7 +2676,7 @@
       <c r="B52" t="s">
         <v>44</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="3">
         <v>145.02</v>
       </c>
       <c r="D52">
@@ -2672,15 +2691,15 @@
         <v>34</v>
       </c>
       <c r="C53" s="2">
-        <f>SUM(C52:C52)</f>
+        <f>SUM(C52)</f>
         <v>0</v>
       </c>
       <c r="D53" s="2">
-        <f>SUM(D52:D52)</f>
+        <f>SUM(D52)</f>
         <v>0</v>
       </c>
       <c r="E53" s="2">
-        <f>SUM(E52:E52)</f>
+        <f>SUM(E52)</f>
         <v>0</v>
       </c>
     </row>
@@ -2704,8 +2723,9 @@
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="B58">
-        <v>154.5</v>
+      <c r="B58" s="2">
+        <f>SUM(C65)</f>
+        <v>0</v>
       </c>
       <c r="C58">
         <v>232.8</v>
@@ -2769,7 +2789,7 @@
       <c r="B65" t="s">
         <v>47</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="3">
         <v>154.5</v>
       </c>
       <c r="D65">
@@ -2784,15 +2804,15 @@
         <v>34</v>
       </c>
       <c r="C66" s="2">
-        <f>SUM(C65:C65)</f>
+        <f>SUM(C65)</f>
         <v>0</v>
       </c>
       <c r="D66" s="2">
-        <f>SUM(D65:D65)</f>
+        <f>SUM(D65)</f>
         <v>0</v>
       </c>
       <c r="E66" s="2">
-        <f>SUM(E65:E65)</f>
+        <f>SUM(E65)</f>
         <v>0</v>
       </c>
     </row>
@@ -2816,8 +2836,9 @@
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="B71">
-        <v>449</v>
+      <c r="B71" s="2">
+        <f>SUM(C78,C79)</f>
+        <v>0</v>
       </c>
       <c r="C71">
         <v>237.6</v>
@@ -2881,7 +2902,7 @@
       <c r="B78" t="s">
         <v>50</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="3">
         <v>309</v>
       </c>
       <c r="D78">
@@ -2895,7 +2916,7 @@
       <c r="B79" t="s">
         <v>51</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="3">
         <v>140</v>
       </c>
       <c r="D79">
@@ -2910,15 +2931,15 @@
         <v>34</v>
       </c>
       <c r="C80" s="2">
-        <f>SUM(C79:C78)</f>
+        <f>SUM(C78,C79)</f>
         <v>0</v>
       </c>
       <c r="D80" s="2">
-        <f>SUM(D79:D78)</f>
+        <f>SUM(D78,D79)</f>
         <v>0</v>
       </c>
       <c r="E80" s="2">
-        <f>SUM(E79:E78)</f>
+        <f>SUM(E78,E79)</f>
         <v>0</v>
       </c>
     </row>
@@ -2942,8 +2963,9 @@
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="B85">
-        <v>305.24</v>
+      <c r="B85" s="2">
+        <f>SUM(C92,C93,C94)</f>
+        <v>0</v>
       </c>
       <c r="C85">
         <v>230.4</v>
@@ -3007,7 +3029,7 @@
       <c r="B92" t="s">
         <v>54</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="3">
         <v>128.1</v>
       </c>
       <c r="D92">
@@ -3021,7 +3043,7 @@
       <c r="B93" t="s">
         <v>55</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="3">
         <v>53.64</v>
       </c>
       <c r="D93">
@@ -3035,7 +3057,7 @@
       <c r="B94" t="s">
         <v>56</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="3">
         <v>123.5</v>
       </c>
       <c r="D94">
@@ -3050,15 +3072,15 @@
         <v>34</v>
       </c>
       <c r="C95" s="2">
-        <f>SUM(C94:C92)</f>
+        <f>SUM(C92,C93,C94)</f>
         <v>0</v>
       </c>
       <c r="D95" s="2">
-        <f>SUM(D94:D92)</f>
+        <f>SUM(D92,D93,D94)</f>
         <v>0</v>
       </c>
       <c r="E95" s="2">
-        <f>SUM(E94:E92)</f>
+        <f>SUM(E92,E93,E94)</f>
         <v>0</v>
       </c>
     </row>
@@ -3082,8 +3104,9 @@
       </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="B100">
-        <v>486.73</v>
+      <c r="B100" s="2">
+        <f>SUM(C107,C108,C109)</f>
+        <v>0</v>
       </c>
       <c r="C100">
         <v>212.4</v>
@@ -3147,7 +3170,7 @@
       <c r="B107" t="s">
         <v>59</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="3">
         <v>280.88</v>
       </c>
       <c r="D107">
@@ -3161,7 +3184,7 @@
       <c r="B108" t="s">
         <v>60</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="3">
         <v>73.85</v>
       </c>
       <c r="D108">
@@ -3175,7 +3198,7 @@
       <c r="B109" t="s">
         <v>61</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="3">
         <v>132</v>
       </c>
       <c r="D109">
@@ -3190,15 +3213,15 @@
         <v>34</v>
       </c>
       <c r="C110" s="2">
-        <f>SUM(C109:C107)</f>
+        <f>SUM(C107,C108,C109)</f>
         <v>0</v>
       </c>
       <c r="D110" s="2">
-        <f>SUM(D109:D107)</f>
+        <f>SUM(D107,D108,D109)</f>
         <v>0</v>
       </c>
       <c r="E110" s="2">
-        <f>SUM(E109:E107)</f>
+        <f>SUM(E107,E108,E109)</f>
         <v>0</v>
       </c>
     </row>
@@ -3222,8 +3245,9 @@
       </c>
     </row>
     <row r="115" spans="1:6">
-      <c r="B115">
-        <v>668.2</v>
+      <c r="B115" s="2">
+        <f>SUM(C122,C123,C124,C125,C126,C127)</f>
+        <v>0</v>
       </c>
       <c r="C115">
         <v>240</v>
@@ -3287,7 +3311,7 @@
       <c r="B122" t="s">
         <v>65</v>
       </c>
-      <c r="C122">
+      <c r="C122" s="3">
         <v>70</v>
       </c>
       <c r="D122">
@@ -3301,7 +3325,7 @@
       <c r="B123" t="s">
         <v>66</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="3">
         <v>147</v>
       </c>
       <c r="D123">
@@ -3315,7 +3339,7 @@
       <c r="B124" t="s">
         <v>67</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="3">
         <v>214</v>
       </c>
       <c r="D124">
@@ -3329,7 +3353,7 @@
       <c r="B125" t="s">
         <v>68</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="3">
         <v>183</v>
       </c>
       <c r="D125">
@@ -3343,7 +3367,7 @@
       <c r="B126" t="s">
         <v>69</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="3">
         <v>3</v>
       </c>
       <c r="D126">
@@ -3357,7 +3381,7 @@
       <c r="B127" t="s">
         <v>70</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="3">
         <v>51.2</v>
       </c>
       <c r="D127">
@@ -3372,15 +3396,15 @@
         <v>34</v>
       </c>
       <c r="C128" s="2">
-        <f>SUM(C127:C122)</f>
+        <f>SUM(C122,C123,C124,C125,C126,C127)</f>
         <v>0</v>
       </c>
       <c r="D128" s="2">
-        <f>SUM(D127:D122)</f>
+        <f>SUM(D122,D123,D124,D125,D126,D127)</f>
         <v>0</v>
       </c>
       <c r="E128" s="2">
-        <f>SUM(E127:E122)</f>
+        <f>SUM(E122,E123,E124,E125,E126,E127)</f>
         <v>0</v>
       </c>
     </row>
@@ -3404,8 +3428,9 @@
       </c>
     </row>
     <row r="133" spans="1:6">
-      <c r="B133">
-        <v>147.2</v>
+      <c r="B133" s="2">
+        <f>SUM(C140)</f>
+        <v>0</v>
       </c>
       <c r="C133">
         <v>259.2</v>
@@ -3469,7 +3494,7 @@
       <c r="B140" t="s">
         <v>73</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="3">
         <v>147.2</v>
       </c>
       <c r="D140">
@@ -3484,15 +3509,15 @@
         <v>34</v>
       </c>
       <c r="C141" s="2">
-        <f>SUM(C140:C140)</f>
+        <f>SUM(C140)</f>
         <v>0</v>
       </c>
       <c r="D141" s="2">
-        <f>SUM(D140:D140)</f>
+        <f>SUM(D140)</f>
         <v>0</v>
       </c>
       <c r="E141" s="2">
-        <f>SUM(E140:E140)</f>
+        <f>SUM(E140)</f>
         <v>0</v>
       </c>
     </row>
@@ -3516,8 +3541,9 @@
       </c>
     </row>
     <row r="146" spans="1:6">
-      <c r="B146">
-        <v>137.6</v>
+      <c r="B146" s="2">
+        <f>SUM(C153)</f>
+        <v>0</v>
       </c>
       <c r="C146">
         <v>237.6</v>
@@ -3581,7 +3607,7 @@
       <c r="B153" t="s">
         <v>75</v>
       </c>
-      <c r="C153">
+      <c r="C153" s="3">
         <v>137.6</v>
       </c>
       <c r="D153">
@@ -3596,15 +3622,15 @@
         <v>34</v>
       </c>
       <c r="C154" s="2">
-        <f>SUM(C153:C153)</f>
+        <f>SUM(C153)</f>
         <v>0</v>
       </c>
       <c r="D154" s="2">
-        <f>SUM(D153:D153)</f>
+        <f>SUM(D153)</f>
         <v>0</v>
       </c>
       <c r="E154" s="2">
-        <f>SUM(E153:E153)</f>
+        <f>SUM(E153)</f>
         <v>0</v>
       </c>
     </row>
@@ -3628,8 +3654,9 @@
       </c>
     </row>
     <row r="159" spans="1:6">
-      <c r="B159">
-        <v>134.5</v>
+      <c r="B159" s="2">
+        <f>SUM(C166)</f>
+        <v>0</v>
       </c>
       <c r="C159">
         <v>240</v>
@@ -3693,7 +3720,7 @@
       <c r="B166" t="s">
         <v>77</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="3">
         <v>134.5</v>
       </c>
       <c r="D166">
@@ -3708,15 +3735,15 @@
         <v>34</v>
       </c>
       <c r="C167" s="2">
-        <f>SUM(C166:C166)</f>
+        <f>SUM(C166)</f>
         <v>0</v>
       </c>
       <c r="D167" s="2">
-        <f>SUM(D166:D166)</f>
+        <f>SUM(D166)</f>
         <v>0</v>
       </c>
       <c r="E167" s="2">
-        <f>SUM(E166:E166)</f>
+        <f>SUM(E166)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>